<commit_message>
include new vars in 2_recode
</commit_message>
<xml_diff>
--- a/output/metadata_recode.xlsx
+++ b/output/metadata_recode.xlsx
@@ -732,7 +732,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_3</t>
+          <t>perper_p_delito_pronostico_2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Robo o hurto de algún objeto dejado dentro del vehículo o parte de él</t>
+          <t>Robo o hurto de su vehículo o portonazo</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_4</t>
+          <t>perper_p_delito_pronostico_3</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Vandalismo o daño a su vivienda o vehículo</t>
+          <t>Robo o hurto de algún objeto dejado dentro del vehículo o parte de él</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_6</t>
+          <t>perper_p_delito_pronostico_4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Hurto</t>
+          <t>Vandalismo o daño a su vivienda o vehículo</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_8</t>
+          <t>perper_p_delito_pronostico_6</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Amenazas o extorsión</t>
+          <t>Hurto</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_2</t>
+          <t>perper_p_delito_pronostico_5</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Robo o hurto de su vehículo o portonazo</t>
+          <t>Robo o asalto, como robo con violencia, cogoteo, robo por sorpresa o lanzazo</t>
         </is>
       </c>
     </row>
@@ -948,7 +948,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_5</t>
+          <t>perper_p_delito_pronostico_7</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -958,7 +958,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Robo o asalto, como robo con violencia, cogoteo, robo por sorpresa o lanzazo</t>
+          <t>Agresiones físicas o lesiones</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>perper_p_delito_pronostico_7</t>
+          <t>perper_p_delito_pronostico_8</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -985,7 +985,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Agresiones físicas o lesiones</t>
+          <t>Amenazas o extorsión</t>
         </is>
       </c>
     </row>

</xml_diff>